<commit_message>
Update app.py and other files
</commit_message>
<xml_diff>
--- a/data/IK_Konj+Destatis_HWWI.xlsx
+++ b/data/IK_Konj+Destatis_HWWI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l.mueller\Documents\FileCloud\Team Folders\IK_Server\Wirtschaft\statistische Daten\ik-dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB37F8F4-C147-4BCC-903B-97E3ACFD487D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0D9DA7-A472-413A-A243-257B4FFEBBF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,16 +28,16 @@
     <t>Monat</t>
   </si>
   <si>
-    <t>Index_Preisentwicklung Energy raw materials</t>
+    <t>Index_Preisentwicklung Energierohstoffe</t>
   </si>
   <si>
-    <t>Index_Preisentwicklung Coal</t>
+    <t>Index_Preisentwicklung Kohle</t>
   </si>
   <si>
-    <t>Index_Preisentwicklung Crude oil</t>
+    <t>Index_Preisentwicklung Rohöl</t>
   </si>
   <si>
-    <t>Index_Preisentwicklung Natural gas</t>
+    <t>Index_Preisentwicklung Erdgas</t>
   </si>
   <si>
     <t>WZ CODE</t>
@@ -475,13 +475,10 @@
   <dimension ref="A1:X41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P41" sqref="P41:X41"/>
+      <selection activeCell="X41" sqref="P41:X41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Daten im data-Ordner aktualisieren
</commit_message>
<xml_diff>
--- a/data/IK_Konj+Destatis_HWWI.xlsx
+++ b/data/IK_Konj+Destatis_HWWI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l.mueller\Documents\FileCloud\Team Folders\IK_Server\Wirtschaft\statistische Daten\ik-dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0D9DA7-A472-413A-A243-257B4FFEBBF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF77DF9-441F-423F-BA89-D78955D9639B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="3660" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="30">
   <si>
     <t>Jahr</t>
   </si>
@@ -472,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X41"/>
+  <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X41" sqref="P41:X41"/>
+    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
+      <selection activeCell="X45" sqref="X45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3361,6 +3361,41 @@
         <v>-53.8</v>
       </c>
     </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2025</v>
+      </c>
+      <c r="B42" t="s">
+        <v>24</v>
+      </c>
+      <c r="G42" t="s">
+        <v>25</v>
+      </c>
+      <c r="H42" t="s">
+        <v>26</v>
+      </c>
+      <c r="I42">
+        <v>-17.39130434782609</v>
+      </c>
+      <c r="J42">
+        <v>-43.478260869565219</v>
+      </c>
+      <c r="K42">
+        <v>-9.8901098901098905</v>
+      </c>
+      <c r="L42">
+        <v>5.4347826086956523</v>
+      </c>
+      <c r="M42">
+        <v>-7.608695652173914</v>
+      </c>
+      <c r="N42">
+        <v>1.086956521739129</v>
+      </c>
+      <c r="O42">
+        <v>-66.304347826086953</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update app with plotly dpendency
</commit_message>
<xml_diff>
--- a/data/IK_Konj+Destatis_HWWI.xlsx
+++ b/data/IK_Konj+Destatis_HWWI.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X42"/>
+  <dimension ref="A1:W43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,80 +476,75 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>Index_Absatz</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>Index_Beschäftigtenzahl</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Index_Ertrag</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Index_Exporte</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Index_Rohstoffverfügbarkeit</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Index_Umsatz</t>
-        </is>
-      </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Index_Verkaufspreise (Branchenprodukte)</t>
+          <t>Index_Wirtschaftslage</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Index_Wirtschaftslage</t>
+          <t>Betriebe</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Betriebe</t>
+          <t>Beschäftigte</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Beschäftigte</t>
+          <t>Geleistete Arbeitsstunden</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Geleistete Arbeitsstunden</t>
+          <t>Bruttolohn- und -gehaltssumme</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Bruttolohn- und -gehaltssumme</t>
+          <t>Umsatz</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Umsatz</t>
+          <t>Inlandsumsatz</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>Inlandsumsatz</t>
+          <t>Auslandsumsatz</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>Auslandsumsatz</t>
+          <t>Auslandsumsatz mit der Eurozone</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>Auslandsumsatz mit der Eurozone</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Auslandsumsatz mit dem sonstigen Ausland</t>
         </is>
@@ -587,47 +582,42 @@
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
-      <c r="J2" t="n">
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="n">
         <v>-4.5</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>1.5</v>
       </c>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="n">
-        <v>16.5</v>
-      </c>
+      <c r="M2" t="inlineStr"/>
       <c r="N2" t="n">
-        <v>-27.8</v>
+        <v>29.3</v>
       </c>
       <c r="O2" t="n">
-        <v>29.3</v>
+        <v>494.3333333333333</v>
       </c>
       <c r="P2" t="n">
-        <v>494.3333333333333</v>
+        <v>85415.66666666667</v>
       </c>
       <c r="Q2" t="n">
-        <v>85415.66666666667</v>
+        <v>34801667</v>
       </c>
       <c r="R2" t="n">
-        <v>34801667</v>
+        <v>812034667</v>
       </c>
       <c r="S2" t="n">
-        <v>812034667</v>
+        <v>5093306000</v>
       </c>
       <c r="T2" t="n">
-        <v>5093306000</v>
+        <v>2846582001</v>
       </c>
       <c r="U2" t="n">
-        <v>2846582001</v>
+        <v>2246724000</v>
       </c>
       <c r="V2" t="n">
-        <v>2246724000</v>
+        <v>1363936667</v>
       </c>
       <c r="W2" t="n">
-        <v>1363936667</v>
-      </c>
-      <c r="X2" t="n">
         <v>882786333</v>
       </c>
     </row>
@@ -663,47 +653,42 @@
         </is>
       </c>
       <c r="I3" t="inlineStr"/>
-      <c r="J3" t="n">
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="n">
         <v>-11.5</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>14.7</v>
       </c>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="n">
-        <v>30</v>
-      </c>
+      <c r="M3" t="inlineStr"/>
       <c r="N3" t="n">
-        <v>4.6</v>
+        <v>58.5</v>
       </c>
       <c r="O3" t="n">
-        <v>58.5</v>
+        <v>494.6666666666667</v>
       </c>
       <c r="P3" t="n">
-        <v>494.6666666666667</v>
+        <v>87143.33333333333</v>
       </c>
       <c r="Q3" t="n">
-        <v>87143.33333333333</v>
+        <v>34417001</v>
       </c>
       <c r="R3" t="n">
-        <v>34417001</v>
+        <v>886895333</v>
       </c>
       <c r="S3" t="n">
-        <v>886895333</v>
+        <v>5312760333</v>
       </c>
       <c r="T3" t="n">
-        <v>5312760333</v>
+        <v>2968539000</v>
       </c>
       <c r="U3" t="n">
-        <v>2968539000</v>
+        <v>2344222334</v>
       </c>
       <c r="V3" t="n">
-        <v>2344222334</v>
+        <v>1422852333</v>
       </c>
       <c r="W3" t="n">
-        <v>1422852333</v>
-      </c>
-      <c r="X3" t="n">
         <v>921369999</v>
       </c>
     </row>
@@ -739,47 +724,42 @@
         </is>
       </c>
       <c r="I4" t="inlineStr"/>
-      <c r="J4" t="n">
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="n">
         <v>-33.9</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>-4.6</v>
       </c>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="n">
-        <v>12.7</v>
-      </c>
+      <c r="M4" t="inlineStr"/>
       <c r="N4" t="n">
-        <v>43.5</v>
+        <v>60.2</v>
       </c>
       <c r="O4" t="n">
-        <v>60.2</v>
+        <v>494.3333333333333</v>
       </c>
       <c r="P4" t="n">
-        <v>494.3333333333333</v>
+        <v>88792.33333333333</v>
       </c>
       <c r="Q4" t="n">
-        <v>88792.33333333333</v>
+        <v>35328334</v>
       </c>
       <c r="R4" t="n">
-        <v>35328334</v>
+        <v>854039666</v>
       </c>
       <c r="S4" t="n">
-        <v>854039666</v>
+        <v>5371702666</v>
       </c>
       <c r="T4" t="n">
-        <v>5371702666</v>
+        <v>3051743667</v>
       </c>
       <c r="U4" t="n">
-        <v>3051743667</v>
+        <v>2319959999</v>
       </c>
       <c r="V4" t="n">
-        <v>2319959999</v>
+        <v>1402910000</v>
       </c>
       <c r="W4" t="n">
-        <v>1402910000</v>
-      </c>
-      <c r="X4" t="n">
         <v>917048334</v>
       </c>
     </row>
@@ -815,47 +795,42 @@
         </is>
       </c>
       <c r="I5" t="inlineStr"/>
-      <c r="J5" t="n">
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="n">
         <v>-4.9</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>4</v>
       </c>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="n">
-        <v>11.8</v>
-      </c>
+      <c r="M5" t="inlineStr"/>
       <c r="N5" t="n">
-        <v>-21.8</v>
+        <v>55.3</v>
       </c>
       <c r="O5" t="n">
-        <v>55.3</v>
+        <v>493.6666666666667</v>
       </c>
       <c r="P5" t="n">
-        <v>493.6666666666667</v>
+        <v>88520.66666666667</v>
       </c>
       <c r="Q5" t="n">
-        <v>88520.66666666667</v>
+        <v>34910000</v>
       </c>
       <c r="R5" t="n">
-        <v>34910000</v>
+        <v>976991000</v>
       </c>
       <c r="S5" t="n">
-        <v>976991000</v>
+        <v>5002082333</v>
       </c>
       <c r="T5" t="n">
-        <v>5002082333</v>
+        <v>2797713334</v>
       </c>
       <c r="U5" t="n">
-        <v>2797713334</v>
+        <v>2204367001</v>
       </c>
       <c r="V5" t="n">
-        <v>2204367001</v>
+        <v>1333176334</v>
       </c>
       <c r="W5" t="n">
-        <v>1333176334</v>
-      </c>
-      <c r="X5" t="n">
         <v>871193334</v>
       </c>
     </row>
@@ -891,47 +866,42 @@
         </is>
       </c>
       <c r="I6" t="inlineStr"/>
-      <c r="J6" t="n">
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="n">
         <v>2.8</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>11.3</v>
       </c>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="n">
-        <v>29.4</v>
-      </c>
+      <c r="M6" t="inlineStr"/>
       <c r="N6" t="n">
-        <v>12.8</v>
+        <v>70.59999999999999</v>
       </c>
       <c r="O6" t="n">
-        <v>70.59999999999999</v>
+        <v>503.6666666666667</v>
       </c>
       <c r="P6" t="n">
-        <v>503.6666666666667</v>
+        <v>89736</v>
       </c>
       <c r="Q6" t="n">
-        <v>89736</v>
+        <v>36504333</v>
       </c>
       <c r="R6" t="n">
-        <v>36504333</v>
+        <v>870135000</v>
       </c>
       <c r="S6" t="n">
-        <v>870135000</v>
+        <v>5264862666</v>
       </c>
       <c r="T6" t="n">
-        <v>5264862666</v>
+        <v>2940092666</v>
       </c>
       <c r="U6" t="n">
-        <v>2940092666</v>
+        <v>2324770000</v>
       </c>
       <c r="V6" t="n">
-        <v>2324770000</v>
+        <v>1428560667</v>
       </c>
       <c r="W6" t="n">
-        <v>1428560667</v>
-      </c>
-      <c r="X6" t="n">
         <v>896210333</v>
       </c>
     </row>
@@ -967,47 +937,42 @@
         </is>
       </c>
       <c r="I7" t="inlineStr"/>
-      <c r="J7" t="n">
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="n">
         <v>-6.9</v>
       </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
         <v>8</v>
       </c>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="n">
-        <v>20.6</v>
-      </c>
+      <c r="M7" t="inlineStr"/>
       <c r="N7" t="n">
-        <v>7.9</v>
+        <v>62.7</v>
       </c>
       <c r="O7" t="n">
-        <v>62.7</v>
+        <v>508.6666666666667</v>
       </c>
       <c r="P7" t="n">
-        <v>508.6666666666667</v>
+        <v>90386</v>
       </c>
       <c r="Q7" t="n">
-        <v>90386</v>
+        <v>36793667</v>
       </c>
       <c r="R7" t="n">
-        <v>36793667</v>
+        <v>946337999</v>
       </c>
       <c r="S7" t="n">
-        <v>946337999</v>
+        <v>5644707667</v>
       </c>
       <c r="T7" t="n">
-        <v>5644707667</v>
+        <v>3178824667</v>
       </c>
       <c r="U7" t="n">
-        <v>3178824667</v>
+        <v>2465883667</v>
       </c>
       <c r="V7" t="n">
-        <v>2465883667</v>
+        <v>1496121000</v>
       </c>
       <c r="W7" t="n">
-        <v>1496121000</v>
-      </c>
-      <c r="X7" t="n">
         <v>969759000</v>
       </c>
     </row>
@@ -1043,47 +1008,42 @@
         </is>
       </c>
       <c r="I8" t="inlineStr"/>
-      <c r="J8" t="n">
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="n">
         <v>-14.5</v>
       </c>
-      <c r="K8" t="n">
+      <c r="L8" t="n">
         <v>4.5</v>
       </c>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="n">
-        <v>10.7</v>
-      </c>
+      <c r="M8" t="inlineStr"/>
       <c r="N8" t="n">
-        <v>4.5</v>
+        <v>72.5</v>
       </c>
       <c r="O8" t="n">
-        <v>72.5</v>
+        <v>510</v>
       </c>
       <c r="P8" t="n">
-        <v>510</v>
+        <v>91594.66666666669</v>
       </c>
       <c r="Q8" t="n">
-        <v>91594.66666666669</v>
+        <v>36339000</v>
       </c>
       <c r="R8" t="n">
-        <v>36339000</v>
+        <v>902081000</v>
       </c>
       <c r="S8" t="n">
-        <v>902081000</v>
+        <v>5586796001</v>
       </c>
       <c r="T8" t="n">
-        <v>5586796001</v>
+        <v>3188010666</v>
       </c>
       <c r="U8" t="n">
-        <v>3188010666</v>
+        <v>2398785667</v>
       </c>
       <c r="V8" t="n">
-        <v>2398785667</v>
+        <v>1436498334</v>
       </c>
       <c r="W8" t="n">
-        <v>1436498334</v>
-      </c>
-      <c r="X8" t="n">
         <v>962288334</v>
       </c>
     </row>
@@ -1119,47 +1079,42 @@
         </is>
       </c>
       <c r="I9" t="inlineStr"/>
-      <c r="J9" t="n">
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="n">
         <v>-8</v>
       </c>
-      <c r="K9" t="n">
+      <c r="L9" t="n">
         <v>2.3</v>
       </c>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="n">
-        <v>22.1</v>
-      </c>
+      <c r="M9" t="inlineStr"/>
       <c r="N9" t="n">
-        <v>2.3</v>
+        <v>60.9</v>
       </c>
       <c r="O9" t="n">
-        <v>60.9</v>
+        <v>509</v>
       </c>
       <c r="P9" t="n">
-        <v>509</v>
+        <v>91318.66666666669</v>
       </c>
       <c r="Q9" t="n">
-        <v>91318.66666666669</v>
+        <v>35379667</v>
       </c>
       <c r="R9" t="n">
-        <v>35379667</v>
+        <v>1023019999</v>
       </c>
       <c r="S9" t="n">
-        <v>1023019999</v>
+        <v>5179956333</v>
       </c>
       <c r="T9" t="n">
-        <v>5179956333</v>
+        <v>2901878667</v>
       </c>
       <c r="U9" t="n">
-        <v>2901878667</v>
+        <v>2278077666</v>
       </c>
       <c r="V9" t="n">
-        <v>2278077666</v>
+        <v>1357997333</v>
       </c>
       <c r="W9" t="n">
-        <v>1357997333</v>
-      </c>
-      <c r="X9" t="n">
         <v>920080001</v>
       </c>
     </row>
@@ -1195,47 +1150,42 @@
         </is>
       </c>
       <c r="I10" t="inlineStr"/>
-      <c r="J10" t="n">
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="n">
         <v>2</v>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
         <v>12.2</v>
       </c>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="n">
-        <v>26.3</v>
-      </c>
+      <c r="M10" t="inlineStr"/>
       <c r="N10" t="n">
-        <v>21.2</v>
+        <v>70</v>
       </c>
       <c r="O10" t="n">
-        <v>70</v>
+        <v>510.6666666666667</v>
       </c>
       <c r="P10" t="n">
-        <v>510.6666666666667</v>
+        <v>90882.66666666669</v>
       </c>
       <c r="Q10" t="n">
-        <v>90882.66666666669</v>
+        <v>37728334</v>
       </c>
       <c r="R10" t="n">
-        <v>37728334</v>
+        <v>905791666</v>
       </c>
       <c r="S10" t="n">
-        <v>905791666</v>
+        <v>5554466000</v>
       </c>
       <c r="T10" t="n">
-        <v>5554466000</v>
+        <v>3043362666</v>
       </c>
       <c r="U10" t="n">
-        <v>3043362666</v>
+        <v>2511104000</v>
       </c>
       <c r="V10" t="n">
-        <v>2511104000</v>
+        <v>1523806667</v>
       </c>
       <c r="W10" t="n">
-        <v>1523806667</v>
-      </c>
-      <c r="X10" t="n">
         <v>987298333</v>
       </c>
     </row>
@@ -1271,47 +1221,42 @@
         </is>
       </c>
       <c r="I11" t="inlineStr"/>
-      <c r="J11" t="n">
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="n">
         <v>-23.5</v>
       </c>
-      <c r="K11" t="n">
+      <c r="L11" t="n">
         <v>-4</v>
       </c>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="n">
-        <v>19.6</v>
-      </c>
+      <c r="M11" t="inlineStr"/>
       <c r="N11" t="n">
-        <v>56.4</v>
+        <v>78.40000000000001</v>
       </c>
       <c r="O11" t="n">
-        <v>78.40000000000001</v>
+        <v>515.3333333333334</v>
       </c>
       <c r="P11" t="n">
-        <v>515.3333333333334</v>
+        <v>91548.66666666669</v>
       </c>
       <c r="Q11" t="n">
-        <v>91548.66666666669</v>
+        <v>36063000</v>
       </c>
       <c r="R11" t="n">
-        <v>36063000</v>
+        <v>982136667</v>
       </c>
       <c r="S11" t="n">
-        <v>982136667</v>
+        <v>5721324333</v>
       </c>
       <c r="T11" t="n">
-        <v>5721324333</v>
+        <v>3125315001</v>
       </c>
       <c r="U11" t="n">
-        <v>3125315001</v>
+        <v>2596007667</v>
       </c>
       <c r="V11" t="n">
-        <v>2596007667</v>
+        <v>1554673667</v>
       </c>
       <c r="W11" t="n">
-        <v>1554673667</v>
-      </c>
-      <c r="X11" t="n">
         <v>1041335000</v>
       </c>
     </row>
@@ -1347,47 +1292,42 @@
         </is>
       </c>
       <c r="I12" t="inlineStr"/>
-      <c r="J12" t="n">
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="n">
         <v>0</v>
       </c>
-      <c r="K12" t="n">
+      <c r="L12" t="n">
         <v>2.1</v>
       </c>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="n">
-        <v>4.3</v>
-      </c>
+      <c r="M12" t="inlineStr"/>
       <c r="N12" t="n">
-        <v>-3.2</v>
+        <v>88.3</v>
       </c>
       <c r="O12" t="n">
-        <v>88.3</v>
+        <v>513</v>
       </c>
       <c r="P12" t="n">
-        <v>513</v>
+        <v>92896.33333333331</v>
       </c>
       <c r="Q12" t="n">
-        <v>92896.33333333331</v>
+        <v>36435333</v>
       </c>
       <c r="R12" t="n">
-        <v>36435333</v>
+        <v>923190001</v>
       </c>
       <c r="S12" t="n">
-        <v>923190001</v>
+        <v>5706937667</v>
       </c>
       <c r="T12" t="n">
-        <v>5706937667</v>
+        <v>3187001334</v>
       </c>
       <c r="U12" t="n">
-        <v>3187001334</v>
+        <v>2519937333</v>
       </c>
       <c r="V12" t="n">
-        <v>2519937333</v>
+        <v>1481948333</v>
       </c>
       <c r="W12" t="n">
-        <v>1481948333</v>
-      </c>
-      <c r="X12" t="n">
         <v>1037990667</v>
       </c>
     </row>
@@ -1423,47 +1363,42 @@
         </is>
       </c>
       <c r="I13" t="inlineStr"/>
-      <c r="J13" t="n">
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="n">
         <v>-12</v>
       </c>
-      <c r="K13" t="n">
+      <c r="L13" t="n">
         <v>9.1</v>
       </c>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="n">
-        <v>25.7</v>
-      </c>
+      <c r="M13" t="inlineStr"/>
       <c r="N13" t="n">
-        <v>23.2</v>
+        <v>86.09999999999999</v>
       </c>
       <c r="O13" t="n">
-        <v>86.09999999999999</v>
+        <v>512.3333333333334</v>
       </c>
       <c r="P13" t="n">
-        <v>512.3333333333334</v>
+        <v>92995</v>
       </c>
       <c r="Q13" t="n">
-        <v>92995</v>
+        <v>35387000</v>
       </c>
       <c r="R13" t="n">
-        <v>35387000</v>
+        <v>1073667999</v>
       </c>
       <c r="S13" t="n">
-        <v>1073667999</v>
+        <v>5313750333</v>
       </c>
       <c r="T13" t="n">
-        <v>5313750333</v>
+        <v>2905312667</v>
       </c>
       <c r="U13" t="n">
-        <v>2905312667</v>
+        <v>2408438000</v>
       </c>
       <c r="V13" t="n">
-        <v>2408438000</v>
+        <v>1442275999</v>
       </c>
       <c r="W13" t="n">
-        <v>1442275999</v>
-      </c>
-      <c r="X13" t="n">
         <v>966161334</v>
       </c>
     </row>
@@ -1499,47 +1434,42 @@
         </is>
       </c>
       <c r="I14" t="inlineStr"/>
-      <c r="J14" t="n">
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="n">
         <v>-5</v>
       </c>
-      <c r="K14" t="n">
+      <c r="L14" t="n">
         <v>15</v>
       </c>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="n">
-        <v>35.6</v>
-      </c>
+      <c r="M14" t="inlineStr"/>
       <c r="N14" t="n">
-        <v>40</v>
+        <v>89.09999999999999</v>
       </c>
       <c r="O14" t="n">
-        <v>89.09999999999999</v>
+        <v>510</v>
       </c>
       <c r="P14" t="n">
-        <v>510</v>
+        <v>95069.66666666669</v>
       </c>
       <c r="Q14" t="n">
-        <v>95069.66666666669</v>
+        <v>38554333</v>
       </c>
       <c r="R14" t="n">
-        <v>38554333</v>
+        <v>975321667</v>
       </c>
       <c r="S14" t="n">
-        <v>975321667</v>
+        <v>5795561667</v>
       </c>
       <c r="T14" t="n">
-        <v>5795561667</v>
+        <v>3151074001</v>
       </c>
       <c r="U14" t="n">
-        <v>3151074001</v>
+        <v>2644488667</v>
       </c>
       <c r="V14" t="n">
-        <v>2644488667</v>
+        <v>1597820666</v>
       </c>
       <c r="W14" t="n">
-        <v>1597820666</v>
-      </c>
-      <c r="X14" t="n">
         <v>1046669667</v>
       </c>
     </row>
@@ -1575,47 +1505,42 @@
         </is>
       </c>
       <c r="I15" t="inlineStr"/>
-      <c r="J15" t="n">
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="n">
         <v>9.800000000000001</v>
       </c>
-      <c r="K15" t="n">
+      <c r="L15" t="n">
         <v>19.8</v>
       </c>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="n">
-        <v>33.7</v>
-      </c>
+      <c r="M15" t="inlineStr"/>
       <c r="N15" t="n">
-        <v>39.8</v>
+        <v>85.5</v>
       </c>
       <c r="O15" t="n">
-        <v>85.5</v>
+        <v>512.6666666666666</v>
       </c>
       <c r="P15" t="n">
-        <v>512.6666666666666</v>
+        <v>95527</v>
       </c>
       <c r="Q15" t="n">
-        <v>95527</v>
+        <v>37477667</v>
       </c>
       <c r="R15" t="n">
-        <v>37477667</v>
+        <v>1041839667</v>
       </c>
       <c r="S15" t="n">
-        <v>1041839667</v>
+        <v>5980455333</v>
       </c>
       <c r="T15" t="n">
-        <v>5980455333</v>
+        <v>3268191000</v>
       </c>
       <c r="U15" t="n">
-        <v>3268191000</v>
+        <v>2712264333</v>
       </c>
       <c r="V15" t="n">
-        <v>2712264333</v>
+        <v>1627374667</v>
       </c>
       <c r="W15" t="n">
-        <v>1627374667</v>
-      </c>
-      <c r="X15" t="n">
         <v>1084889666</v>
       </c>
     </row>
@@ -1651,47 +1576,42 @@
         </is>
       </c>
       <c r="I16" t="inlineStr"/>
-      <c r="J16" t="n">
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="n">
         <v>-20.3</v>
       </c>
-      <c r="K16" t="n">
+      <c r="L16" t="n">
         <v>-7</v>
       </c>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="n">
-        <v>11.9</v>
-      </c>
+      <c r="M16" t="inlineStr"/>
       <c r="N16" t="n">
-        <v>34.7</v>
+        <v>78</v>
       </c>
       <c r="O16" t="n">
-        <v>78</v>
+        <v>514.6666666666666</v>
       </c>
       <c r="P16" t="n">
-        <v>514.6666666666666</v>
+        <v>97077</v>
       </c>
       <c r="Q16" t="n">
-        <v>97077</v>
+        <v>37658333</v>
       </c>
       <c r="R16" t="n">
-        <v>37658333</v>
+        <v>988303000</v>
       </c>
       <c r="S16" t="n">
-        <v>988303000</v>
+        <v>5848516667</v>
       </c>
       <c r="T16" t="n">
-        <v>5848516667</v>
+        <v>3289888333</v>
       </c>
       <c r="U16" t="n">
-        <v>3289888333</v>
+        <v>2558627666</v>
       </c>
       <c r="V16" t="n">
-        <v>2558627666</v>
+        <v>1507515333</v>
       </c>
       <c r="W16" t="n">
-        <v>1507515333</v>
-      </c>
-      <c r="X16" t="n">
         <v>1051112334</v>
       </c>
     </row>
@@ -1727,47 +1647,42 @@
         </is>
       </c>
       <c r="I17" t="inlineStr"/>
-      <c r="J17" t="n">
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="n">
         <v>-21.7</v>
       </c>
-      <c r="K17" t="n">
+      <c r="L17" t="n">
         <v>2.8</v>
       </c>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="n">
-        <v>15</v>
-      </c>
+      <c r="M17" t="inlineStr"/>
       <c r="N17" t="n">
-        <v>22.6</v>
+        <v>75</v>
       </c>
       <c r="O17" t="n">
-        <v>75</v>
+        <v>513.6666666666666</v>
       </c>
       <c r="P17" t="n">
-        <v>513.6666666666666</v>
+        <v>96858.33333333331</v>
       </c>
       <c r="Q17" t="n">
-        <v>96858.33333333331</v>
+        <v>36775667</v>
       </c>
       <c r="R17" t="n">
-        <v>36775667</v>
+        <v>1149175333</v>
       </c>
       <c r="S17" t="n">
-        <v>1149175333</v>
+        <v>5427716000</v>
       </c>
       <c r="T17" t="n">
-        <v>5427716000</v>
+        <v>2991843333</v>
       </c>
       <c r="U17" t="n">
-        <v>2991843333</v>
+        <v>2435873666</v>
       </c>
       <c r="V17" t="n">
-        <v>2435873666</v>
+        <v>1448474333</v>
       </c>
       <c r="W17" t="n">
-        <v>1448474333</v>
-      </c>
-      <c r="X17" t="n">
         <v>987400666</v>
       </c>
     </row>
@@ -1803,47 +1718,42 @@
         </is>
       </c>
       <c r="I18" t="inlineStr"/>
-      <c r="J18" t="n">
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="n">
         <v>-13.1</v>
       </c>
-      <c r="K18" t="n">
+      <c r="L18" t="n">
         <v>-4.6</v>
       </c>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="n">
-        <v>0.9</v>
-      </c>
+      <c r="M18" t="inlineStr"/>
       <c r="N18" t="n">
-        <v>19.6</v>
+        <v>59.4</v>
       </c>
       <c r="O18" t="n">
-        <v>59.4</v>
+        <v>513.6666666666666</v>
       </c>
       <c r="P18" t="n">
-        <v>513.6666666666666</v>
+        <v>94968.33333333331</v>
       </c>
       <c r="Q18" t="n">
-        <v>94968.33333333331</v>
+        <v>38536999</v>
       </c>
       <c r="R18" t="n">
-        <v>38536999</v>
+        <v>970536000</v>
       </c>
       <c r="S18" t="n">
-        <v>970536000</v>
+        <v>5890009000</v>
       </c>
       <c r="T18" t="n">
-        <v>5890009000</v>
+        <v>3240303000</v>
       </c>
       <c r="U18" t="n">
-        <v>3240303000</v>
+        <v>2649704667</v>
       </c>
       <c r="V18" t="n">
-        <v>2649704667</v>
+        <v>1607776667</v>
       </c>
       <c r="W18" t="n">
-        <v>1607776667</v>
-      </c>
-      <c r="X18" t="n">
         <v>1041927334</v>
       </c>
     </row>
@@ -1879,47 +1789,42 @@
         </is>
       </c>
       <c r="I19" t="inlineStr"/>
-      <c r="J19" t="n">
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="n">
         <v>-20</v>
       </c>
-      <c r="K19" t="n">
+      <c r="L19" t="n">
         <v>-12.2</v>
       </c>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="n">
-        <v>9.5</v>
-      </c>
+      <c r="M19" t="inlineStr"/>
       <c r="N19" t="n">
-        <v>9.5</v>
+        <v>42.9</v>
       </c>
       <c r="O19" t="n">
-        <v>42.9</v>
+        <v>520</v>
       </c>
       <c r="P19" t="n">
-        <v>520</v>
+        <v>95082.33333333331</v>
       </c>
       <c r="Q19" t="n">
-        <v>95082.33333333331</v>
+        <v>36891000</v>
       </c>
       <c r="R19" t="n">
-        <v>36891000</v>
+        <v>1053273000</v>
       </c>
       <c r="S19" t="n">
-        <v>1053273000</v>
+        <v>5856515000</v>
       </c>
       <c r="T19" t="n">
-        <v>5856515000</v>
+        <v>3226729334</v>
       </c>
       <c r="U19" t="n">
-        <v>3226729334</v>
+        <v>2629786001</v>
       </c>
       <c r="V19" t="n">
-        <v>2629786001</v>
+        <v>1576261334</v>
       </c>
       <c r="W19" t="n">
-        <v>1576261334</v>
-      </c>
-      <c r="X19" t="n">
         <v>1053524667</v>
       </c>
     </row>
@@ -1955,47 +1860,42 @@
         </is>
       </c>
       <c r="I20" t="inlineStr"/>
-      <c r="J20" t="n">
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="n">
         <v>-17.4</v>
       </c>
-      <c r="K20" t="n">
+      <c r="L20" t="n">
         <v>-20.3</v>
       </c>
-      <c r="L20" t="inlineStr"/>
-      <c r="M20" t="n">
-        <v>-11.6</v>
-      </c>
+      <c r="M20" t="inlineStr"/>
       <c r="N20" t="n">
-        <v>-5.8</v>
+        <v>32.5</v>
       </c>
       <c r="O20" t="n">
-        <v>32.5</v>
+        <v>520</v>
       </c>
       <c r="P20" t="n">
-        <v>520</v>
+        <v>95791.33333333331</v>
       </c>
       <c r="Q20" t="n">
-        <v>95791.33333333331</v>
+        <v>37470000</v>
       </c>
       <c r="R20" t="n">
-        <v>37470000</v>
+        <v>992028334</v>
       </c>
       <c r="S20" t="n">
-        <v>992028334</v>
+        <v>5824154667</v>
       </c>
       <c r="T20" t="n">
-        <v>5824154667</v>
+        <v>3245235666</v>
       </c>
       <c r="U20" t="n">
-        <v>3245235666</v>
+        <v>2578917333</v>
       </c>
       <c r="V20" t="n">
-        <v>2578917333</v>
+        <v>1509165666</v>
       </c>
       <c r="W20" t="n">
-        <v>1509165666</v>
-      </c>
-      <c r="X20" t="n">
         <v>1069753333</v>
       </c>
     </row>
@@ -2031,47 +1931,42 @@
         </is>
       </c>
       <c r="I21" t="inlineStr"/>
-      <c r="J21" t="n">
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="n">
         <v>-39.3</v>
       </c>
-      <c r="K21" t="n">
+      <c r="L21" t="n">
         <v>-35.1</v>
       </c>
-      <c r="L21" t="inlineStr"/>
-      <c r="M21" t="n">
-        <v>-37.5</v>
-      </c>
+      <c r="M21" t="inlineStr"/>
       <c r="N21" t="n">
-        <v>-18.9</v>
+        <v>-7.1</v>
       </c>
       <c r="O21" t="n">
-        <v>-7.1</v>
+        <v>519.6666666666666</v>
       </c>
       <c r="P21" t="n">
-        <v>519.6666666666666</v>
+        <v>94913.33333333331</v>
       </c>
       <c r="Q21" t="n">
-        <v>94913.33333333331</v>
+        <v>35702666</v>
       </c>
       <c r="R21" t="n">
-        <v>35702666</v>
+        <v>1128682667</v>
       </c>
       <c r="S21" t="n">
-        <v>1128682667</v>
+        <v>5237315001</v>
       </c>
       <c r="T21" t="n">
-        <v>5237315001</v>
+        <v>2841992334</v>
       </c>
       <c r="U21" t="n">
-        <v>2841992334</v>
+        <v>2395322667</v>
       </c>
       <c r="V21" t="n">
-        <v>2395322667</v>
+        <v>1414362667</v>
       </c>
       <c r="W21" t="n">
-        <v>1414362667</v>
-      </c>
-      <c r="X21" t="n">
         <v>980959000</v>
       </c>
     </row>
@@ -2107,47 +2002,42 @@
         </is>
       </c>
       <c r="I22" t="inlineStr"/>
-      <c r="J22" t="n">
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="n">
         <v>-25.2</v>
       </c>
-      <c r="K22" t="n">
+      <c r="L22" t="n">
         <v>-15.5</v>
       </c>
-      <c r="L22" t="inlineStr"/>
-      <c r="M22" t="n">
-        <v>-6.3</v>
-      </c>
+      <c r="M22" t="inlineStr"/>
       <c r="N22" t="n">
-        <v>-20.7</v>
+        <v>4.5</v>
       </c>
       <c r="O22" t="n">
-        <v>4.5</v>
+        <v>510.6666666666667</v>
       </c>
       <c r="P22" t="n">
-        <v>510.6666666666667</v>
+        <v>91198.66666666669</v>
       </c>
       <c r="Q22" t="n">
-        <v>91198.66666666669</v>
+        <v>36901333</v>
       </c>
       <c r="R22" t="n">
-        <v>36901333</v>
+        <v>962999334</v>
       </c>
       <c r="S22" t="n">
-        <v>962999334</v>
+        <v>5709659333</v>
       </c>
       <c r="T22" t="n">
-        <v>5709659333</v>
+        <v>3135780667</v>
       </c>
       <c r="U22" t="n">
-        <v>3135780667</v>
+        <v>2573877666</v>
       </c>
       <c r="V22" t="n">
-        <v>2573877666</v>
+        <v>1539225000</v>
       </c>
       <c r="W22" t="n">
-        <v>1539225000</v>
-      </c>
-      <c r="X22" t="n">
         <v>1034652667</v>
       </c>
     </row>
@@ -2182,52 +2072,47 @@
           <t>IK Kunststoffverpackungen</t>
         </is>
       </c>
-      <c r="I23" t="n">
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="n">
         <v>-25.1</v>
       </c>
-      <c r="J23" t="n">
+      <c r="K23" t="n">
         <v>-43.3</v>
       </c>
-      <c r="K23" t="n">
+      <c r="L23" t="n">
         <v>-50.5</v>
       </c>
-      <c r="L23" t="n">
+      <c r="M23" t="n">
         <v>-14.4</v>
       </c>
-      <c r="M23" t="n">
+      <c r="N23" t="n">
         <v>-34.6</v>
       </c>
-      <c r="N23" t="n">
-        <v>-27.9</v>
-      </c>
       <c r="O23" t="n">
-        <v>-34.6</v>
+        <v>511</v>
       </c>
       <c r="P23" t="n">
-        <v>511</v>
+        <v>90453.66666666669</v>
       </c>
       <c r="Q23" t="n">
-        <v>90453.66666666669</v>
+        <v>33309667</v>
       </c>
       <c r="R23" t="n">
-        <v>33309667</v>
+        <v>972206999</v>
       </c>
       <c r="S23" t="n">
-        <v>972206999</v>
+        <v>5263440001</v>
       </c>
       <c r="T23" t="n">
-        <v>5263440001</v>
+        <v>2968302334</v>
       </c>
       <c r="U23" t="n">
-        <v>2968302334</v>
+        <v>2295139333</v>
       </c>
       <c r="V23" t="n">
-        <v>2295139333</v>
+        <v>1348063000</v>
       </c>
       <c r="W23" t="n">
-        <v>1348063000</v>
-      </c>
-      <c r="X23" t="n">
         <v>947075000</v>
       </c>
     </row>
@@ -2262,52 +2147,47 @@
           <t>IK Kunststoffverpackungen</t>
         </is>
       </c>
-      <c r="I24" t="n">
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="n">
         <v>-32.7</v>
       </c>
-      <c r="J24" t="n">
+      <c r="K24" t="n">
         <v>-44.9</v>
       </c>
-      <c r="K24" t="n">
+      <c r="L24" t="n">
         <v>-37.1</v>
       </c>
-      <c r="L24" t="n">
+      <c r="M24" t="n">
         <v>12.1</v>
       </c>
-      <c r="M24" t="n">
-        <v>-30.8</v>
-      </c>
       <c r="N24" t="n">
-        <v>-28</v>
+        <v>-65.40000000000001</v>
       </c>
       <c r="O24" t="n">
-        <v>-65.40000000000001</v>
+        <v>509.3333333333333</v>
       </c>
       <c r="P24" t="n">
-        <v>509.3333333333333</v>
+        <v>90486.33333333331</v>
       </c>
       <c r="Q24" t="n">
-        <v>90486.33333333331</v>
+        <v>34561333</v>
       </c>
       <c r="R24" t="n">
-        <v>34561333</v>
+        <v>943230333</v>
       </c>
       <c r="S24" t="n">
-        <v>943230333</v>
+        <v>5455198666</v>
       </c>
       <c r="T24" t="n">
-        <v>5455198666</v>
+        <v>3009501667</v>
       </c>
       <c r="U24" t="n">
-        <v>3009501667</v>
+        <v>2445697667</v>
       </c>
       <c r="V24" t="n">
-        <v>2445697667</v>
+        <v>1436132334</v>
       </c>
       <c r="W24" t="n">
-        <v>1436132334</v>
-      </c>
-      <c r="X24" t="n">
         <v>1009566333</v>
       </c>
     </row>
@@ -2342,52 +2222,47 @@
           <t>IK Kunststoffverpackungen</t>
         </is>
       </c>
-      <c r="I25" t="n">
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="n">
         <v>-25</v>
       </c>
-      <c r="J25" t="n">
+      <c r="K25" t="n">
         <v>-30.2</v>
       </c>
-      <c r="K25" t="n">
+      <c r="L25" t="n">
         <v>-25</v>
       </c>
-      <c r="L25" t="n">
+      <c r="M25" t="n">
         <v>7.8</v>
       </c>
-      <c r="M25" t="n">
-        <v>-7.8</v>
-      </c>
       <c r="N25" t="n">
-        <v>-23.3</v>
+        <v>-36.2</v>
       </c>
       <c r="O25" t="n">
-        <v>-36.2</v>
+        <v>507.6666666666667</v>
       </c>
       <c r="P25" t="n">
-        <v>507.6666666666667</v>
+        <v>90082</v>
       </c>
       <c r="Q25" t="n">
-        <v>90082</v>
+        <v>34245666</v>
       </c>
       <c r="R25" t="n">
-        <v>34245666</v>
+        <v>1109092667</v>
       </c>
       <c r="S25" t="n">
-        <v>1109092667</v>
+        <v>5318301334</v>
       </c>
       <c r="T25" t="n">
-        <v>5318301334</v>
+        <v>2884399667</v>
       </c>
       <c r="U25" t="n">
-        <v>2884399667</v>
+        <v>2433902667</v>
       </c>
       <c r="V25" t="n">
-        <v>2433902667</v>
+        <v>1430003666</v>
       </c>
       <c r="W25" t="n">
-        <v>1430003666</v>
-      </c>
-      <c r="X25" t="n">
         <v>1003897334</v>
       </c>
     </row>
@@ -2422,52 +2297,47 @@
           <t>IK Kunststoffverpackungen</t>
         </is>
       </c>
-      <c r="I26" t="n">
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="n">
         <v>-4.9</v>
       </c>
-      <c r="J26" t="n">
+      <c r="K26" t="n">
         <v>-22.5</v>
       </c>
-      <c r="K26" t="n">
+      <c r="L26" t="n">
         <v>-17.6</v>
       </c>
-      <c r="L26" t="n">
+      <c r="M26" t="n">
         <v>-47.1</v>
       </c>
-      <c r="M26" t="n">
-        <v>2.9</v>
-      </c>
       <c r="N26" t="n">
-        <v>24.5</v>
+        <v>-15.8</v>
       </c>
       <c r="O26" t="n">
-        <v>-15.8</v>
+        <v>502</v>
       </c>
       <c r="P26" t="n">
-        <v>502</v>
+        <v>90729.66666666669</v>
       </c>
       <c r="Q26" t="n">
-        <v>90729.66666666669</v>
+        <v>36965999</v>
       </c>
       <c r="R26" t="n">
-        <v>36965999</v>
+        <v>974585334</v>
       </c>
       <c r="S26" t="n">
-        <v>974585334</v>
+        <v>5976957334</v>
       </c>
       <c r="T26" t="n">
-        <v>5976957334</v>
+        <v>3244216334</v>
       </c>
       <c r="U26" t="n">
-        <v>3244216334</v>
+        <v>2732742000</v>
       </c>
       <c r="V26" t="n">
-        <v>2732742000</v>
+        <v>1596298000</v>
       </c>
       <c r="W26" t="n">
-        <v>1596298000</v>
-      </c>
-      <c r="X26" t="n">
         <v>1136444667</v>
       </c>
     </row>
@@ -2502,52 +2372,47 @@
           <t>IK Kunststoffverpackungen</t>
         </is>
       </c>
-      <c r="I27" t="n">
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="n">
         <v>0</v>
       </c>
-      <c r="J27" t="n">
+      <c r="K27" t="n">
         <v>-67.7</v>
       </c>
-      <c r="K27" t="n">
+      <c r="L27" t="n">
         <v>-11.1</v>
       </c>
-      <c r="L27" t="n">
+      <c r="M27" t="n">
         <v>-82.8</v>
       </c>
-      <c r="M27" t="n">
-        <v>12.1</v>
-      </c>
       <c r="N27" t="n">
-        <v>86.90000000000001</v>
+        <v>5.1</v>
       </c>
       <c r="O27" t="n">
-        <v>5.1</v>
+        <v>502.3333333333333</v>
       </c>
       <c r="P27" t="n">
-        <v>502.3333333333333</v>
+        <v>90940.66666666669</v>
       </c>
       <c r="Q27" t="n">
-        <v>90940.66666666669</v>
+        <v>35490667</v>
       </c>
       <c r="R27" t="n">
-        <v>35490667</v>
+        <v>1054579999</v>
       </c>
       <c r="S27" t="n">
-        <v>1054579999</v>
+        <v>6521004667</v>
       </c>
       <c r="T27" t="n">
-        <v>6521004667</v>
+        <v>3571823999</v>
       </c>
       <c r="U27" t="n">
-        <v>3571823999</v>
+        <v>2949181333</v>
       </c>
       <c r="V27" t="n">
-        <v>2949181333</v>
+        <v>1697369667</v>
       </c>
       <c r="W27" t="n">
-        <v>1697369667</v>
-      </c>
-      <c r="X27" t="n">
         <v>1251811667</v>
       </c>
     </row>
@@ -2582,52 +2447,47 @@
           <t>IK Kunststoffverpackungen</t>
         </is>
       </c>
-      <c r="I28" t="n">
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="n">
         <v>17.3</v>
       </c>
-      <c r="J28" t="n">
+      <c r="K28" t="n">
         <v>-31.6</v>
       </c>
-      <c r="K28" t="n">
+      <c r="L28" t="n">
         <v>-4.2</v>
       </c>
-      <c r="L28" t="n">
+      <c r="M28" t="n">
         <v>2</v>
       </c>
-      <c r="M28" t="n">
-        <v>17.3</v>
-      </c>
       <c r="N28" t="n">
-        <v>52</v>
+        <v>43.9</v>
       </c>
       <c r="O28" t="n">
-        <v>43.9</v>
+        <v>502</v>
       </c>
       <c r="P28" t="n">
-        <v>502</v>
+        <v>91740.66666666669</v>
       </c>
       <c r="Q28" t="n">
-        <v>91740.66666666669</v>
+        <v>35435001</v>
       </c>
       <c r="R28" t="n">
-        <v>35435001</v>
+        <v>992792000</v>
       </c>
       <c r="S28" t="n">
-        <v>992792000</v>
+        <v>6682369000</v>
       </c>
       <c r="T28" t="n">
-        <v>6682369000</v>
+        <v>3692664667</v>
       </c>
       <c r="U28" t="n">
-        <v>3692664667</v>
+        <v>2989704333</v>
       </c>
       <c r="V28" t="n">
-        <v>2989704333</v>
+        <v>1687728333</v>
       </c>
       <c r="W28" t="n">
-        <v>1687728333</v>
-      </c>
-      <c r="X28" t="n">
         <v>1301976000</v>
       </c>
     </row>
@@ -2662,52 +2522,47 @@
           <t>IK Kunststoffverpackungen</t>
         </is>
       </c>
-      <c r="I29" t="n">
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="n">
         <v>6.8</v>
       </c>
-      <c r="J29" t="n">
+      <c r="K29" t="n">
         <v>-22.7</v>
       </c>
-      <c r="K29" t="n">
+      <c r="L29" t="n">
         <v>-8.1</v>
       </c>
-      <c r="L29" t="n">
+      <c r="M29" t="n">
         <v>-2.3</v>
       </c>
-      <c r="M29" t="n">
-        <v>1.1</v>
-      </c>
       <c r="N29" t="n">
-        <v>30.7</v>
+        <v>33</v>
       </c>
       <c r="O29" t="n">
-        <v>33</v>
+        <v>501</v>
       </c>
       <c r="P29" t="n">
-        <v>501</v>
+        <v>92002.66666666669</v>
       </c>
       <c r="Q29" t="n">
-        <v>92002.66666666669</v>
+        <v>34791000</v>
       </c>
       <c r="R29" t="n">
-        <v>34791000</v>
+        <v>1135991667</v>
       </c>
       <c r="S29" t="n">
-        <v>1135991667</v>
+        <v>6255121333</v>
       </c>
       <c r="T29" t="n">
-        <v>6255121333</v>
+        <v>3363693000</v>
       </c>
       <c r="U29" t="n">
-        <v>3363693000</v>
+        <v>2891427666</v>
       </c>
       <c r="V29" t="n">
-        <v>2891427666</v>
+        <v>1658191667</v>
       </c>
       <c r="W29" t="n">
-        <v>1658191667</v>
-      </c>
-      <c r="X29" t="n">
         <v>1233235667</v>
       </c>
     </row>
@@ -2742,52 +2597,47 @@
           <t>IK Kunststoffverpackungen</t>
         </is>
       </c>
-      <c r="I30" t="n">
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="n">
         <v>0.8</v>
       </c>
-      <c r="J30" t="n">
+      <c r="K30" t="n">
         <v>-41.2</v>
       </c>
-      <c r="K30" t="n">
+      <c r="L30" t="n">
         <v>-7.7</v>
       </c>
-      <c r="L30" t="n">
+      <c r="M30" t="n">
         <v>-25.2</v>
       </c>
-      <c r="M30" t="n">
+      <c r="N30" t="n">
         <v>5.9</v>
       </c>
-      <c r="N30" t="n">
-        <v>74.8</v>
-      </c>
       <c r="O30" t="n">
-        <v>5.9</v>
+        <v>507</v>
       </c>
       <c r="P30" t="n">
-        <v>507</v>
+        <v>92544</v>
       </c>
       <c r="Q30" t="n">
-        <v>92544</v>
+        <v>37085334</v>
       </c>
       <c r="R30" t="n">
-        <v>37085334</v>
+        <v>1003298000</v>
       </c>
       <c r="S30" t="n">
-        <v>1003298000</v>
+        <v>7260732999</v>
       </c>
       <c r="T30" t="n">
-        <v>7260732999</v>
+        <v>3952320667</v>
       </c>
       <c r="U30" t="n">
-        <v>3952320667</v>
+        <v>3308410666</v>
       </c>
       <c r="V30" t="n">
-        <v>3308410666</v>
+        <v>1942118333</v>
       </c>
       <c r="W30" t="n">
-        <v>1942118333</v>
-      </c>
-      <c r="X30" t="n">
         <v>1366293000</v>
       </c>
     </row>
@@ -2822,52 +2672,47 @@
           <t>IK Kunststoffverpackungen</t>
         </is>
       </c>
-      <c r="I31" t="n">
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="n">
         <v>-6.7</v>
       </c>
-      <c r="J31" t="n">
+      <c r="K31" t="n">
         <v>-75</v>
       </c>
-      <c r="K31" t="n">
+      <c r="L31" t="n">
         <v>-45.5</v>
       </c>
-      <c r="L31" t="n">
+      <c r="M31" t="n">
         <v>-76.90000000000001</v>
       </c>
-      <c r="M31" t="n">
-        <v>-24.3</v>
-      </c>
       <c r="N31" t="n">
-        <v>95.2</v>
+        <v>-12.6</v>
       </c>
       <c r="O31" t="n">
-        <v>-12.6</v>
+        <v>509.6666666666667</v>
       </c>
       <c r="P31" t="n">
-        <v>509.6666666666667</v>
+        <v>93034.33333333331</v>
       </c>
       <c r="Q31" t="n">
-        <v>93034.33333333331</v>
+        <v>35705334</v>
       </c>
       <c r="R31" t="n">
-        <v>35705334</v>
+        <v>1100923000</v>
       </c>
       <c r="S31" t="n">
-        <v>1100923000</v>
+        <v>7571556001</v>
       </c>
       <c r="T31" t="n">
-        <v>7571556001</v>
+        <v>4122349001</v>
       </c>
       <c r="U31" t="n">
-        <v>4122349001</v>
+        <v>3449206333</v>
       </c>
       <c r="V31" t="n">
-        <v>3449206333</v>
+        <v>2028426334</v>
       </c>
       <c r="W31" t="n">
-        <v>2028426334</v>
-      </c>
-      <c r="X31" t="n">
         <v>1420781667</v>
       </c>
     </row>
@@ -2902,52 +2747,47 @@
           <t>IK Kunststoffverpackungen</t>
         </is>
       </c>
-      <c r="I32" t="n">
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="n">
         <v>-0.9</v>
       </c>
-      <c r="J32" t="n">
+      <c r="K32" t="n">
         <v>-46.8</v>
       </c>
-      <c r="K32" t="n">
+      <c r="L32" t="n">
         <v>-34.3</v>
       </c>
-      <c r="L32" t="n">
+      <c r="M32" t="n">
         <v>-17.4</v>
       </c>
-      <c r="M32" t="n">
-        <v>-23.9</v>
-      </c>
       <c r="N32" t="n">
-        <v>55.6</v>
+        <v>-14.7</v>
       </c>
       <c r="O32" t="n">
-        <v>-14.7</v>
+        <v>508.6666666666667</v>
       </c>
       <c r="P32" t="n">
-        <v>508.6666666666667</v>
+        <v>93600.33333333331</v>
       </c>
       <c r="Q32" t="n">
-        <v>93600.33333333331</v>
+        <v>35585333</v>
       </c>
       <c r="R32" t="n">
-        <v>35585333</v>
+        <v>1033791666</v>
       </c>
       <c r="S32" t="n">
-        <v>1033791666</v>
+        <v>7266519333</v>
       </c>
       <c r="T32" t="n">
-        <v>7266519333</v>
+        <v>4026950334</v>
       </c>
       <c r="U32" t="n">
-        <v>4026950334</v>
+        <v>3239569333</v>
       </c>
       <c r="V32" t="n">
-        <v>3239569333</v>
+        <v>1838788333</v>
       </c>
       <c r="W32" t="n">
-        <v>1838788333</v>
-      </c>
-      <c r="X32" t="n">
         <v>1400780000</v>
       </c>
     </row>
@@ -2982,52 +2822,47 @@
           <t>IK Kunststoffverpackungen</t>
         </is>
       </c>
-      <c r="I33" t="n">
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="n">
         <v>-27.7</v>
       </c>
-      <c r="J33" t="n">
+      <c r="K33" t="n">
         <v>-77.09999999999999</v>
       </c>
-      <c r="K33" t="n">
+      <c r="L33" t="n">
         <v>-61.4</v>
       </c>
-      <c r="L33" t="n">
+      <c r="M33" t="n">
         <v>4.8</v>
       </c>
-      <c r="M33" t="n">
-        <v>-65.09999999999999</v>
-      </c>
       <c r="N33" t="n">
-        <v>26.5</v>
+        <v>-47</v>
       </c>
       <c r="O33" t="n">
-        <v>-47</v>
+        <v>508.3333333333333</v>
       </c>
       <c r="P33" t="n">
-        <v>508.3333333333333</v>
+        <v>93135.33333333331</v>
       </c>
       <c r="Q33" t="n">
-        <v>93135.33333333331</v>
+        <v>34132667</v>
       </c>
       <c r="R33" t="n">
-        <v>34132667</v>
+        <v>1188628667</v>
       </c>
       <c r="S33" t="n">
-        <v>1188628667</v>
+        <v>6450587000</v>
       </c>
       <c r="T33" t="n">
-        <v>6450587000</v>
+        <v>3496869000</v>
       </c>
       <c r="U33" t="n">
-        <v>3496869000</v>
+        <v>2953718000</v>
       </c>
       <c r="V33" t="n">
-        <v>2953718000</v>
+        <v>1678906000</v>
       </c>
       <c r="W33" t="n">
-        <v>1678906000</v>
-      </c>
-      <c r="X33" t="n">
         <v>1274810999</v>
       </c>
     </row>
@@ -3062,52 +2897,47 @@
           <t>IK Kunststoffverpackungen</t>
         </is>
       </c>
-      <c r="I34" t="n">
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="n">
         <v>-16.2</v>
       </c>
-      <c r="J34" t="n">
+      <c r="K34" t="n">
         <v>-59.8</v>
       </c>
-      <c r="K34" t="n">
+      <c r="L34" t="n">
         <v>-40.8</v>
       </c>
-      <c r="L34" t="n">
+      <c r="M34" t="n">
         <v>21.2</v>
       </c>
-      <c r="M34" t="n">
-        <v>-45.5</v>
-      </c>
       <c r="N34" t="n">
-        <v>15.2</v>
+        <v>-27.3</v>
       </c>
       <c r="O34" t="n">
-        <v>-27.3</v>
+        <v>516</v>
       </c>
       <c r="P34" t="n">
-        <v>516</v>
+        <v>92631</v>
       </c>
       <c r="Q34" t="n">
-        <v>92631</v>
+        <v>37253334</v>
       </c>
       <c r="R34" t="n">
-        <v>37253334</v>
+        <v>1063899000</v>
       </c>
       <c r="S34" t="n">
-        <v>1063899000</v>
+        <v>7023919000</v>
       </c>
       <c r="T34" t="n">
-        <v>7023919000</v>
+        <v>3765564000</v>
       </c>
       <c r="U34" t="n">
-        <v>3765564000</v>
+        <v>3258355000</v>
       </c>
       <c r="V34" t="n">
-        <v>3258355000</v>
+        <v>1933470667</v>
       </c>
       <c r="W34" t="n">
-        <v>1933470667</v>
-      </c>
-      <c r="X34" t="n">
         <v>1324885333</v>
       </c>
     </row>
@@ -3142,52 +2972,47 @@
           <t>IK Kunststoffverpackungen</t>
         </is>
       </c>
-      <c r="I35" t="n">
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="n">
         <v>-23.5</v>
       </c>
-      <c r="J35" t="n">
+      <c r="K35" t="n">
         <v>-57.3</v>
       </c>
-      <c r="K35" t="n">
+      <c r="L35" t="n">
         <v>-42.5</v>
       </c>
-      <c r="L35" t="n">
+      <c r="M35" t="n">
         <v>18.3</v>
       </c>
-      <c r="M35" t="n">
-        <v>-39</v>
-      </c>
       <c r="N35" t="n">
-        <v>-42</v>
+        <v>-20.7</v>
       </c>
       <c r="O35" t="n">
-        <v>-20.7</v>
+        <v>519.6666666666666</v>
       </c>
       <c r="P35" t="n">
-        <v>519.6666666666666</v>
+        <v>92435.66666666669</v>
       </c>
       <c r="Q35" t="n">
-        <v>92435.66666666669</v>
+        <v>34534333</v>
       </c>
       <c r="R35" t="n">
-        <v>34534333</v>
+        <v>1133245666</v>
       </c>
       <c r="S35" t="n">
-        <v>1133245666</v>
+        <v>6583597001</v>
       </c>
       <c r="T35" t="n">
-        <v>6583597001</v>
+        <v>3543930999</v>
       </c>
       <c r="U35" t="n">
-        <v>3543930999</v>
+        <v>3039664333</v>
       </c>
       <c r="V35" t="n">
-        <v>3039664333</v>
+        <v>1804471667</v>
       </c>
       <c r="W35" t="n">
-        <v>1804471667</v>
-      </c>
-      <c r="X35" t="n">
         <v>1235192001</v>
       </c>
     </row>
@@ -3222,52 +3047,47 @@
           <t>IK Kunststoffverpackungen</t>
         </is>
       </c>
-      <c r="I36" t="n">
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="n">
         <v>-32.6</v>
       </c>
-      <c r="J36" t="n">
+      <c r="K36" t="n">
         <v>-57.1</v>
       </c>
-      <c r="K36" t="n">
+      <c r="L36" t="n">
         <v>-30.6</v>
       </c>
-      <c r="L36" t="n">
+      <c r="M36" t="n">
         <v>34.1</v>
       </c>
-      <c r="M36" t="n">
-        <v>-32.6</v>
-      </c>
       <c r="N36" t="n">
-        <v>-61.2</v>
+        <v>-46.5</v>
       </c>
       <c r="O36" t="n">
-        <v>-46.5</v>
+        <v>519</v>
       </c>
       <c r="P36" t="n">
-        <v>519</v>
+        <v>92216.33333333331</v>
       </c>
       <c r="Q36" t="n">
-        <v>92216.33333333331</v>
+        <v>34677667</v>
       </c>
       <c r="R36" t="n">
-        <v>34677667</v>
+        <v>1059254667</v>
       </c>
       <c r="S36" t="n">
-        <v>1059254667</v>
+        <v>6367878001</v>
       </c>
       <c r="T36" t="n">
-        <v>6367878001</v>
+        <v>3462244333</v>
       </c>
       <c r="U36" t="n">
-        <v>3462244333</v>
+        <v>2905634666</v>
       </c>
       <c r="V36" t="n">
-        <v>2905634666</v>
+        <v>1671945667</v>
       </c>
       <c r="W36" t="n">
-        <v>1671945667</v>
-      </c>
-      <c r="X36" t="n">
         <v>1233688000</v>
       </c>
     </row>
@@ -3302,52 +3122,47 @@
           <t>IK Kunststoffverpackungen</t>
         </is>
       </c>
-      <c r="I37" t="n">
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="n">
         <v>-32.6</v>
       </c>
-      <c r="J37" t="n">
+      <c r="K37" t="n">
         <v>-67.40000000000001</v>
       </c>
-      <c r="K37" t="n">
+      <c r="L37" t="n">
         <v>-43.2</v>
       </c>
-      <c r="L37" t="n">
+      <c r="M37" t="n">
         <v>9</v>
       </c>
-      <c r="M37" t="n">
-        <v>-42.7</v>
-      </c>
       <c r="N37" t="n">
-        <v>-30.3</v>
+        <v>-62.9</v>
       </c>
       <c r="O37" t="n">
-        <v>-62.9</v>
+        <v>518</v>
       </c>
       <c r="P37" t="n">
-        <v>518</v>
+        <v>91727.66666666669</v>
       </c>
       <c r="Q37" t="n">
-        <v>91727.66666666669</v>
+        <v>33598333</v>
       </c>
       <c r="R37" t="n">
-        <v>33598333</v>
+        <v>1221556667</v>
       </c>
       <c r="S37" t="n">
-        <v>1221556667</v>
+        <v>5866299334</v>
       </c>
       <c r="T37" t="n">
-        <v>5866299334</v>
+        <v>3118449667</v>
       </c>
       <c r="U37" t="n">
-        <v>3118449667</v>
+        <v>2747849000</v>
       </c>
       <c r="V37" t="n">
-        <v>2747849000</v>
+        <v>1591837000</v>
       </c>
       <c r="W37" t="n">
-        <v>1591837000</v>
-      </c>
-      <c r="X37" t="n">
         <v>1156011000</v>
       </c>
     </row>
@@ -3382,52 +3197,47 @@
           <t>IK Kunststoffverpackungen</t>
         </is>
       </c>
-      <c r="I38" t="n">
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="n">
         <v>-28</v>
       </c>
-      <c r="J38" t="n">
+      <c r="K38" t="n">
         <v>-67.3</v>
       </c>
-      <c r="K38" t="n">
+      <c r="L38" t="n">
         <v>-17.8</v>
       </c>
-      <c r="L38" t="n">
+      <c r="M38" t="n">
         <v>13.1</v>
       </c>
-      <c r="M38" t="n">
-        <v>-23.4</v>
-      </c>
       <c r="N38" t="n">
-        <v>-16.8</v>
+        <v>-57</v>
       </c>
       <c r="O38" t="n">
-        <v>-57</v>
+        <v>515.3333333333334</v>
       </c>
       <c r="P38" t="n">
-        <v>515.3333333333334</v>
+        <v>91020.33333333331</v>
       </c>
       <c r="Q38" t="n">
-        <v>91020.33333333331</v>
+        <v>35914000</v>
       </c>
       <c r="R38" t="n">
-        <v>35914000</v>
+        <v>1095762000</v>
       </c>
       <c r="S38" t="n">
-        <v>1095762000</v>
+        <v>6347076666</v>
       </c>
       <c r="T38" t="n">
-        <v>6347076666</v>
+        <v>3326465666</v>
       </c>
       <c r="U38" t="n">
-        <v>3326465666</v>
+        <v>3020612000</v>
       </c>
       <c r="V38" t="n">
-        <v>3020612000</v>
+        <v>1781262667</v>
       </c>
       <c r="W38" t="n">
-        <v>1781262667</v>
-      </c>
-      <c r="X38" t="n">
         <v>1239349000</v>
       </c>
     </row>
@@ -3462,52 +3272,47 @@
           <t>IK Kunststoffverpackungen</t>
         </is>
       </c>
-      <c r="I39" t="n">
+      <c r="I39" t="inlineStr"/>
+      <c r="J39" t="n">
         <v>-18.3</v>
       </c>
-      <c r="J39" t="n">
+      <c r="K39" t="n">
         <v>-52.9</v>
       </c>
-      <c r="K39" t="n">
+      <c r="L39" t="n">
         <v>-19.4</v>
       </c>
-      <c r="L39" t="n">
+      <c r="M39" t="n">
         <v>-16.3</v>
       </c>
-      <c r="M39" t="n">
-        <v>-6.7</v>
-      </c>
       <c r="N39" t="n">
-        <v>18.3</v>
+        <v>-58.7</v>
       </c>
       <c r="O39" t="n">
-        <v>-58.7</v>
+        <v>520.3333333333334</v>
       </c>
       <c r="P39" t="n">
-        <v>520.3333333333334</v>
+        <v>91106.33333333331</v>
       </c>
       <c r="Q39" t="n">
-        <v>91106.33333333331</v>
+        <v>34765333</v>
       </c>
       <c r="R39" t="n">
-        <v>34765333</v>
+        <v>1163913000</v>
       </c>
       <c r="S39" t="n">
-        <v>1163913000</v>
+        <v>6503759666</v>
       </c>
       <c r="T39" t="n">
-        <v>6503759666</v>
+        <v>3432560000</v>
       </c>
       <c r="U39" t="n">
-        <v>3432560000</v>
+        <v>3071200667</v>
       </c>
       <c r="V39" t="n">
-        <v>3071200667</v>
+        <v>1843917333</v>
       </c>
       <c r="W39" t="n">
-        <v>1843917333</v>
-      </c>
-      <c r="X39" t="n">
         <v>1227282333</v>
       </c>
     </row>
@@ -3542,52 +3347,47 @@
           <t>IK Kunststoffverpackungen</t>
         </is>
       </c>
-      <c r="I40" t="n">
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="n">
         <v>-13.7</v>
       </c>
-      <c r="J40" t="n">
+      <c r="K40" t="n">
         <v>-39.2</v>
       </c>
-      <c r="K40" t="n">
+      <c r="L40" t="n">
         <v>-11</v>
       </c>
-      <c r="L40" t="n">
+      <c r="M40" t="n">
         <v>-1</v>
       </c>
-      <c r="M40" t="n">
-        <v>-16.7</v>
-      </c>
       <c r="N40" t="n">
-        <v>-7.8</v>
+        <v>-53.9</v>
       </c>
       <c r="O40" t="n">
-        <v>-53.9</v>
+        <v>519</v>
       </c>
       <c r="P40" t="n">
-        <v>519</v>
+        <v>91500.66666666669</v>
       </c>
       <c r="Q40" t="n">
-        <v>91500.66666666669</v>
+        <v>34787667</v>
       </c>
       <c r="R40" t="n">
-        <v>34787667</v>
+        <v>1095399999</v>
       </c>
       <c r="S40" t="n">
-        <v>1095399999</v>
+        <v>6371018000</v>
       </c>
       <c r="T40" t="n">
-        <v>6371018000</v>
+        <v>3415055333</v>
       </c>
       <c r="U40" t="n">
-        <v>3415055333</v>
+        <v>2955962667</v>
       </c>
       <c r="V40" t="n">
-        <v>2955962667</v>
+        <v>1685432333</v>
       </c>
       <c r="W40" t="n">
-        <v>1685432333</v>
-      </c>
-      <c r="X40" t="n">
         <v>1270530001</v>
       </c>
     </row>
@@ -3622,52 +3422,47 @@
           <t>IK Kunststoffverpackungen</t>
         </is>
       </c>
-      <c r="I41" t="n">
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="n">
         <v>-20.2</v>
       </c>
-      <c r="J41" t="n">
+      <c r="K41" t="n">
         <v>-51.9</v>
       </c>
-      <c r="K41" t="n">
+      <c r="L41" t="n">
         <v>-25.7</v>
       </c>
-      <c r="L41" t="n">
+      <c r="M41" t="n">
         <v>0</v>
       </c>
-      <c r="M41" t="n">
-        <v>-29.8</v>
-      </c>
       <c r="N41" t="n">
-        <v>-3.8</v>
+        <v>-53.8</v>
       </c>
       <c r="O41" t="n">
-        <v>-53.8</v>
+        <v>518.3333333333334</v>
       </c>
       <c r="P41" t="n">
-        <v>518.3333333333334</v>
+        <v>91660</v>
       </c>
       <c r="Q41" t="n">
-        <v>91660</v>
+        <v>33439001</v>
       </c>
       <c r="R41" t="n">
-        <v>33439001</v>
+        <v>1251171000</v>
       </c>
       <c r="S41" t="n">
-        <v>1251171000</v>
+        <v>5800767666</v>
       </c>
       <c r="T41" t="n">
-        <v>5800767666</v>
+        <v>3030831999</v>
       </c>
       <c r="U41" t="n">
-        <v>3030831999</v>
+        <v>2769936000</v>
       </c>
       <c r="V41" t="n">
-        <v>2769936000</v>
+        <v>1595233333</v>
       </c>
       <c r="W41" t="n">
-        <v>1595233333</v>
-      </c>
-      <c r="X41" t="n">
         <v>1174701333</v>
       </c>
     </row>
@@ -3694,27 +3489,23 @@
           <t>IK Kunststoffverpackungen</t>
         </is>
       </c>
-      <c r="I42" t="n">
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="n">
         <v>-17.39130434782609</v>
       </c>
-      <c r="J42" t="n">
+      <c r="K42" t="n">
         <v>-43.47826086956522</v>
       </c>
-      <c r="K42" t="n">
+      <c r="L42" t="n">
         <v>-9.890109890109891</v>
       </c>
-      <c r="L42" t="n">
+      <c r="M42" t="n">
         <v>5.434782608695652</v>
       </c>
-      <c r="M42" t="n">
-        <v>-7.608695652173914</v>
-      </c>
       <c r="N42" t="n">
-        <v>1.086956521739129</v>
-      </c>
-      <c r="O42" t="n">
-        <v>-66.30434782608695</v>
-      </c>
+        <v>-66.304347826087</v>
+      </c>
+      <c r="O42" t="inlineStr"/>
       <c r="P42" t="inlineStr"/>
       <c r="Q42" t="inlineStr"/>
       <c r="R42" t="inlineStr"/>
@@ -3723,7 +3514,55 @@
       <c r="U42" t="inlineStr"/>
       <c r="V42" t="inlineStr"/>
       <c r="W42" t="inlineStr"/>
-      <c r="X42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>2025</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Q2</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>WZ08-2221(2/3) + WZ08-2222</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>IK Kunststoffverpackungen</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="n">
+        <v>-15.2</v>
+      </c>
+      <c r="K43" t="n">
+        <v>-32.4</v>
+      </c>
+      <c r="L43" t="n">
+        <v>-8.699999999999999</v>
+      </c>
+      <c r="M43" t="n">
+        <v>-6.7</v>
+      </c>
+      <c r="N43" t="n">
+        <v>-56.2</v>
+      </c>
+      <c r="O43" t="inlineStr"/>
+      <c r="P43" t="inlineStr"/>
+      <c r="Q43" t="inlineStr"/>
+      <c r="R43" t="inlineStr"/>
+      <c r="S43" t="inlineStr"/>
+      <c r="T43" t="inlineStr"/>
+      <c r="U43" t="inlineStr"/>
+      <c r="V43" t="inlineStr"/>
+      <c r="W43" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>